<commit_message>
Update sesion 1c and workshops
</commit_message>
<xml_diff>
--- a/Sesiones/Sesion-1/Data/maca_meno_perclin.xlsx
+++ b/Sesiones/Sesion-1/Data/maca_meno_perclin.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/74d2a9162288af9c/Cursos Dictados/IETSI-Cursos/Analisis-Datos-R-2022/Presentaciones/Sesion-1/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="154" documentId="8_{6825003D-DBF7-4887-92C1-924B2EFB7D70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E6507F82-9D54-406D-9BC3-00078381F56B}"/>
+  <xr:revisionPtr revIDLastSave="158" documentId="8_{6825003D-DBF7-4887-92C1-924B2EFB7D70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{980F3CAF-58E9-475B-A64A-5293FCA0A449}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{38724DD3-DFE6-4915-8B2F-9589EA5071D6}"/>
+    <workbookView minimized="1" xWindow="12390" yWindow="6585" windowWidth="2400" windowHeight="585" xr2:uid="{38724DD3-DFE6-4915-8B2F-9589EA5071D6}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -567,8 +567,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56119E2F-1B1B-4E65-A8C7-32B4FA3DE043}">
   <dimension ref="A1:M24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -577,8 +577,7 @@
     <col min="2" max="2" width="7.42578125" style="1" customWidth="1"/>
     <col min="3" max="3" width="20.7109375" style="1" customWidth="1"/>
     <col min="4" max="4" width="10.85546875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="7" style="1" customWidth="1"/>
-    <col min="6" max="6" width="9" style="1" customWidth="1"/>
+    <col min="5" max="6" width="12.5703125" style="1" customWidth="1"/>
     <col min="7" max="7" width="12.42578125" style="1" customWidth="1"/>
     <col min="8" max="8" width="11" style="3"/>
     <col min="9" max="9" width="13.7109375" style="3" customWidth="1"/>

</xml_diff>